<commit_message>
feat: Add verify button
</commit_message>
<xml_diff>
--- a/mess_rebate.xlsx
+++ b/mess_rebate.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
   <si>
     <t>Sl.No.</t>
   </si>
@@ -41,6 +41,9 @@
   </si>
   <si>
     <t>Amount to be refunded</t>
+  </si>
+  <si>
+    <t>Verified</t>
   </si>
   <si>
     <t>BTECH</t>
@@ -83,7 +86,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -100,12 +103,15 @@
       <name val="Arial"/>
     </font>
     <font>
+      <b/>
+    </font>
+    <font>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font/>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -116,6 +122,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF0B"/>
         <bgColor rgb="FFFFFF0B"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -139,7 +151,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -152,10 +164,13 @@
     <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -413,101 +428,113 @@
       <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
+      <c r="K1" s="4" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="4">
+      <c r="A2" s="5">
         <v>1.0</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="C2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="D2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="4">
+      <c r="E2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="5">
         <v>8.967570983E9</v>
       </c>
-      <c r="G2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="4">
+      <c r="G2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="5">
         <v>2.367846433443E12</v>
       </c>
-      <c r="I2" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="J2" s="4">
+      <c r="I2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" s="5">
         <v>3000.0</v>
+      </c>
+      <c r="K2" s="5">
+        <v>0.0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="5">
+      <c r="A3" s="6">
         <v>2.0</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="5" t="s">
+      <c r="B3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="5">
+        <v>8.967570983E9</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="5">
+        <v>2.367846433443E12</v>
+      </c>
+      <c r="I3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="4">
-        <v>8.967570983E9</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" s="4">
-        <v>2.367846433443E12</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="J3" s="4">
+      <c r="J3" s="5">
         <v>3000.0</v>
+      </c>
+      <c r="K3" s="5">
+        <v>0.0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="4">
+      <c r="A4" s="5">
         <v>3.0</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="4" t="s">
+      <c r="B4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="D4" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="5">
+      <c r="E4" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="6">
         <v>8.967570983E9</v>
       </c>
-      <c r="G4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" s="4">
+      <c r="G4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="5">
         <v>2.367846433443E12</v>
       </c>
-      <c r="I4" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="J4" s="4">
+      <c r="I4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" s="5">
         <v>3000.0</v>
+      </c>
+      <c r="K4" s="5">
+        <v>1.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>